<commit_message>
Second Commit | Excel is update
</commit_message>
<xml_diff>
--- a/HPV_BrokenLinks/src/main/resources/URL_List.xlsx
+++ b/HPV_BrokenLinks/src/main/resources/URL_List.xlsx
@@ -19,15 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Test URL List</t>
   </si>
   <si>
     <t>https://www.hpv16and18.com/index.html</t>
-  </si>
-  <si>
-    <t>https://lifescience.roche.com/en_in.html</t>
   </si>
   <si>
     <t>https://global.hpv16and18.com/hcp/index.html</t>
@@ -378,10 +375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -401,11 +398,6 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>